<commit_message>
Updated data, figures and started making Omikron plots
</commit_message>
<xml_diff>
--- a/DanskeData/Omikron.xlsx
+++ b/DanskeData/Omikron.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>2021-11-24</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>AntalOmikron</t>
+  </si>
+  <si>
+    <t>Ratio</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +433,7 @@
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -440,8 +443,11 @@
       <c r="C1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,8 +457,12 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>100*C2/B2</f>
+        <v>2.6946914578280787E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -462,8 +472,12 @@
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D14" si="0">100*C3/B3</f>
+        <v>5.1572975760701391E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -473,8 +487,12 @@
       <c r="C4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.15048908954100829</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -484,8 +502,12 @@
       <c r="C5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>7.6550140341923964E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -495,8 +517,12 @@
       <c r="C6">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.28683181225554105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -506,72 +532,122 @@
       <c r="C7">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.24984384759525297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5106</v>
+        <v>5181</v>
       </c>
       <c r="C8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.46323103647944414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>4161</v>
+        <v>4267</v>
       </c>
       <c r="C9">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.8045465198031403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4264</v>
+        <v>4294</v>
       </c>
       <c r="C10">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.4438751746623195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3712</v>
+        <v>4946</v>
       </c>
       <c r="C11">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.5163768701981399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>4992</v>
+      </c>
+      <c r="C12">
+        <v>110</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2.203525641025641</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3544</v>
+      </c>
+      <c r="C13">
+        <v>110</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3.1038374717832955</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>232</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>4.3103448275862073</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Updated data and Omikron plots
</commit_message>
<xml_diff>
--- a/DanskeData/Omikron.xlsx
+++ b/DanskeData/Omikron.xlsx
@@ -423,7 +423,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +473,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D14" si="0">100*C3/B3</f>
+        <f t="shared" ref="D3:D15" si="0">100*C3/B3</f>
         <v>5.1572975760701391E-2</v>
       </c>
     </row>
@@ -602,14 +602,14 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>4992</v>
+        <v>5016</v>
       </c>
       <c r="C12">
         <v>110</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>2.203525641025641</v>
+        <v>2.192982456140351</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -617,14 +617,14 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>3544</v>
+        <v>4582</v>
       </c>
       <c r="C13">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>3.1038374717832955</v>
+        <v>3.2736796158882586</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,14 +632,14 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>232</v>
+        <v>4348</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>189</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>4.3103448275862073</v>
+        <v>4.3468261269549222</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Omikron numbers, now using variant-pdf instead of report...
</commit_message>
<xml_diff>
--- a/DanskeData/Omikron.xlsx
+++ b/DanskeData/Omikron.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>2021-11-24</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>2021-11-23</t>
+  </si>
+  <si>
+    <t>2021-12-08</t>
+  </si>
+  <si>
+    <t>2021-12-09</t>
+  </si>
+  <si>
+    <t>2021-12-10</t>
   </si>
 </sst>
 </file>
@@ -405,7 +414,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="A18:D18"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +464,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D18" si="0">100*C3/B3</f>
+        <f t="shared" ref="D3:D20" si="0">100*C3/B3</f>
         <v>2.1431633090441493E-2</v>
       </c>
     </row>
@@ -509,14 +518,14 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>3813</v>
+        <v>3919</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>7.8678206136900075E-2</v>
+        <v>7.6550140341923964E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -524,14 +533,14 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>3849</v>
+        <v>3835</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.25980774227071968</v>
+        <v>0.28683181225554105</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -539,14 +548,14 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>5048</v>
+        <v>4803</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.19809825673534073</v>
+        <v>0.24984384759525297</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -554,14 +563,14 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>5368</v>
+        <v>5181</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.46572280178837555</v>
+        <v>0.46323103647944414</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -569,14 +578,14 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>4491</v>
+        <v>4267</v>
       </c>
       <c r="C11">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>1.6922734357604097</v>
+        <v>1.8045465198031403</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -584,14 +593,14 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>4528</v>
+        <v>4294</v>
       </c>
       <c r="C12">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>1.3250883392226149</v>
+        <v>1.4438751746623195</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -599,14 +608,14 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>5126</v>
+        <v>4946</v>
       </c>
       <c r="C13">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>1.48263753413968</v>
+        <v>1.5163768701981399</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,14 +623,14 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>5058</v>
+        <v>5089</v>
       </c>
       <c r="C14">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>1.9968366943455911</v>
+        <v>2.1811750835134602</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,14 +638,14 @@
         <v>11</v>
       </c>
       <c r="B15">
-        <v>4768</v>
+        <v>4995</v>
       </c>
       <c r="C15">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>3.5864093959731544</v>
+        <v>3.3433433433433435</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -644,14 +653,14 @@
         <v>12</v>
       </c>
       <c r="B16">
-        <v>7028</v>
+        <v>6762</v>
       </c>
       <c r="C16">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>5.0085372794536145</v>
+        <v>4.9837326234841761</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -659,24 +668,60 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <v>7162</v>
+        <v>7039</v>
       </c>
       <c r="C17">
-        <v>581</v>
+        <v>530</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>8.1122591454900874</v>
+        <v>7.5294786191220346</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>6204</v>
+      </c>
+      <c r="C18">
+        <v>643</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>10.36428110896196</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>4223</v>
+      </c>
+      <c r="C19">
+        <v>501</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>11.863604072933933</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>2912</v>
+      </c>
+      <c r="C20">
+        <v>381</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>13.083791208791208</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>

</xml_diff>

<commit_message>
Various updates with new data and updated Omikron calculations
</commit_message>
<xml_diff>
--- a/DanskeData/Omikron.xlsx
+++ b/DanskeData/Omikron.xlsx
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>2021-11-24</t>
-  </si>
-  <si>
-    <t>2021-11-25</t>
-  </si>
-  <si>
-    <t>2021-11-26</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>2021-11-27</t>
   </si>
@@ -80,12 +71,6 @@
     <t>Ratio</t>
   </si>
   <si>
-    <t>2021-11-22</t>
-  </si>
-  <si>
-    <t>2021-11-23</t>
-  </si>
-  <si>
     <t>2021-12-08</t>
   </si>
   <si>
@@ -93,6 +78,27 @@
   </si>
   <si>
     <t>2021-12-10</t>
+  </si>
+  <si>
+    <t>2021-12-11</t>
+  </si>
+  <si>
+    <t>2021-12-12</t>
+  </si>
+  <si>
+    <t>2021-12-13</t>
+  </si>
+  <si>
+    <t>2021-12-14</t>
+  </si>
+  <si>
+    <t>2021-12-15</t>
+  </si>
+  <si>
+    <t>2021-12-16</t>
+  </si>
+  <si>
+    <t>2021-12-17</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,256 +432,256 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>4470</v>
+        <v>4029</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <f>100*C2/B2</f>
-        <v>2.2371364653243849E-2</v>
+        <f t="shared" ref="D2:D22" si="0">100*C2/B2</f>
+        <v>7.4460163812360383E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>4666</v>
+        <v>4000</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D20" si="0">100*C3/B3</f>
-        <v>2.1431633090441493E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.27500000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3982</v>
+        <v>5034</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <f>100*C4/B4</f>
-        <v>2.5113008538422903E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.23837902264600716</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4059</v>
+        <v>5374</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>9.8546440009854644E-2</v>
+        <v>0.44659471529586897</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>4114</v>
+        <v>4456</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.17015070491006321</v>
+        <v>1.7280071813285458</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>3919</v>
+        <v>4563</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>7.6550140341923964E-2</v>
+        <v>1.3806706114398422</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>3835</v>
+        <v>5161</v>
       </c>
       <c r="C8">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.28683181225554105</v>
+        <v>1.4919589226894012</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>4803</v>
+        <v>5301</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.24984384759525297</v>
+        <v>2.112808903980381</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>5181</v>
+        <v>5176</v>
       </c>
       <c r="C10">
-        <v>24</v>
+        <v>169</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.46323103647944414</v>
+        <v>3.2650695517774344</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>4267</v>
+        <v>7115</v>
       </c>
       <c r="C11">
-        <v>77</v>
+        <v>355</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>1.8045465198031403</v>
+        <v>4.9894588896697121</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>4294</v>
+        <v>7316</v>
       </c>
       <c r="C12">
-        <v>62</v>
+        <v>552</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>1.4438751746623195</v>
+        <v>7.5451066156369597</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>4946</v>
+        <v>6575</v>
       </c>
       <c r="C13">
-        <v>75</v>
+        <v>691</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>1.5163768701981399</v>
+        <v>10.509505703422054</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>5089</v>
+        <v>6536</v>
       </c>
       <c r="C14">
-        <v>111</v>
+        <v>750</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>2.1811750835134602</v>
+        <v>11.474908200734394</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>4995</v>
+        <v>6823</v>
       </c>
       <c r="C15">
-        <v>167</v>
+        <v>897</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>3.3433433433433435</v>
+        <v>13.146709658507987</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>6762</v>
+        <v>6661</v>
       </c>
       <c r="C16">
-        <v>337</v>
+        <v>1113</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>4.9837326234841761</v>
+        <v>16.709202822399039</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>7039</v>
+        <v>7048</v>
       </c>
       <c r="C17">
-        <v>530</v>
+        <v>1557</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>7.5294786191220346</v>
+        <v>22.091373439273553</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -683,14 +689,14 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>6204</v>
+        <v>9864</v>
       </c>
       <c r="C18">
-        <v>643</v>
+        <v>2863</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>10.36428110896196</v>
+        <v>29.024736415247364</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -698,14 +704,14 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>4223</v>
+        <v>11220</v>
       </c>
       <c r="C19">
-        <v>501</v>
+        <v>4372</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>11.863604072933933</v>
+        <v>38.96613190730838</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,21 +719,45 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>2912</v>
+        <v>10981</v>
       </c>
       <c r="C20">
-        <v>381</v>
+        <v>5095</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>13.083791208791208</v>
+        <v>46.398324378471905</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>7605</v>
+      </c>
+      <c r="C21">
+        <v>3480</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>45.759368836291912</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>3770</v>
+      </c>
+      <c r="C22">
+        <v>1632</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>43.289124668435015</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>

</xml_diff>